<commit_message>
Trying with feature method
</commit_message>
<xml_diff>
--- a/Excel Case Study - 2 (1).xlsx
+++ b/Excel Case Study - 2 (1).xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\OneDrive\Desktop\Gitclass\Apache\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C90B86FA-81AA-4389-A0E7-CAD5833DBD2D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F362BB-D9D3-4DB2-AE9D-F9576315937D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="6945" tabRatio="758" activeTab="4" xr2:uid="{79EB00AA-E363-4462-86A0-44CFA398920C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="758" activeTab="3" xr2:uid="{79EB00AA-E363-4462-86A0-44CFA398920C}"/>
   </bookViews>
   <sheets>
     <sheet name="Question 1" sheetId="2" r:id="rId1"/>
@@ -25,18 +25,29 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId9"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="425">
   <si>
     <t>PREFIX</t>
   </si>
@@ -1404,6 +1415,9 @@
   <si>
     <t>Years</t>
   </si>
+  <si>
+    <t>a</t>
+  </si>
 </sst>
 </file>
 
@@ -1411,10 +1425,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="000"/>
-    <numFmt numFmtId="167" formatCode="dd\ mmm\ yyyy"/>
-    <numFmt numFmtId="169" formatCode="0.0\ &quot;kg&quot;"/>
-    <numFmt numFmtId="171" formatCode="[&lt;100000]0.00,&quot;K&quot;;0.0,\ &quot;K&quot;"/>
+    <numFmt numFmtId="165" formatCode="000"/>
+    <numFmt numFmtId="166" formatCode="dd\ mmm\ yyyy"/>
+    <numFmt numFmtId="167" formatCode="0.0\ &quot;kg&quot;"/>
+    <numFmt numFmtId="168" formatCode="[&lt;100000]0.00,&quot;K&quot;;0.0,\ &quot;K&quot;"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -1825,7 +1839,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1840,9 +1854,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1850,14 +1861,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1876,16 +1887,34 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1915,25 +1944,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1957,7 +1967,7 @@
     <worksheetSource ref="A1:S51" sheet="SPORTSMEN"/>
   </cacheSource>
   <cacheFields count="21">
-    <cacheField name="MEMBER ID" numFmtId="166">
+    <cacheField name="MEMBER ID" numFmtId="165">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="50" count="50">
         <n v="1"/>
         <n v="2"/>
@@ -2077,7 +2087,7 @@
     <cacheField name="LASTNAME" numFmtId="0">
       <sharedItems/>
     </cacheField>
-    <cacheField name="BIRTHDATE" numFmtId="167">
+    <cacheField name="BIRTHDATE" numFmtId="166">
       <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1955-07-30T00:00:00" maxDate="1999-08-29T00:00:00" count="50">
         <d v="1997-09-26T00:00:00"/>
         <d v="1992-02-07T00:00:00"/>
@@ -2242,7 +2252,7 @@
         <s v="sobrinho.adriano@.com"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="WEIGHT" numFmtId="169">
+    <cacheField name="WEIGHT" numFmtId="167">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="45.9" maxValue="105.9"/>
     </cacheField>
     <cacheField name="EYECOLOR" numFmtId="0">
@@ -2293,7 +2303,7 @@
         <s v="Swimming"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="SALARY" numFmtId="171">
+    <cacheField name="SALARY" numFmtId="168">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="10241" maxValue="117408"/>
     </cacheField>
     <cacheField name="Quarters" numFmtId="0" databaseField="0">
@@ -3428,16 +3438,16 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3268EFC6-C114-45F5-8FD7-EAF4DF2C4CBA}" name="PivotTable1" cacheId="12" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3268EFC6-C114-45F5-8FD7-EAF4DF2C4CBA}" name="PivotTable1" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B3:D15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="21">
-    <pivotField numFmtId="166" showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField numFmtId="167" showAll="0">
+    <pivotField numFmtId="166" showAll="0">
       <items count="15">
         <item x="0"/>
         <item x="1"/>
@@ -3483,12 +3493,12 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField numFmtId="169" showAll="0"/>
+    <pivotField numFmtId="167" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField numFmtId="171" showAll="0"/>
+    <pivotField numFmtId="168" showAll="0"/>
     <pivotField showAll="0">
       <items count="7">
         <item x="0"/>
@@ -3618,10 +3628,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B445550E-0F9C-4C67-BFA0-F5B790170BB1}" name="PivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B445550E-0F9C-4C67-BFA0-F5B790170BB1}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:H53" firstHeaderRow="1" firstDataRow="1" firstDataCol="8" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="21">
-    <pivotField axis="axisRow" compact="0" numFmtId="166" outline="0" showAll="0" defaultSubtotal="0">
+    <pivotField axis="axisRow" compact="0" numFmtId="165" outline="0" showAll="0" defaultSubtotal="0">
       <items count="50">
         <item x="0"/>
         <item x="1"/>
@@ -3733,7 +3743,7 @@
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" numFmtId="167" outline="0" showAll="0" defaultSubtotal="0">
+    <pivotField compact="0" numFmtId="166" outline="0" showAll="0" defaultSubtotal="0">
       <items count="14">
         <item x="0"/>
         <item x="1"/>
@@ -3839,7 +3849,7 @@
         <item x="11"/>
       </items>
     </pivotField>
-    <pivotField compact="0" numFmtId="169" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" numFmtId="167" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisPage" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
@@ -3884,7 +3894,7 @@
         <item x="4"/>
       </items>
     </pivotField>
-    <pivotField compact="0" numFmtId="171" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" numFmtId="168" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="6">
         <item sd="0" x="0"/>
@@ -4478,9 +4488,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4518,7 +4528,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4624,7 +4634,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4766,7 +4776,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4789,177 +4799,177 @@
   <sheetData>
     <row r="1" spans="2:5" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="44" t="s">
         <v>251</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="41" t="s">
+      <c r="C2" s="45"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="50" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="38"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="42"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="2:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="42" t="s">
         <v>224</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="34"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="43"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="19">
+      <c r="B7" s="18">
         <v>1</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="12">
+      <c r="B8" s="11">
         <v>2</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="12" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="12">
+      <c r="B9" s="11">
         <v>3</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="12" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <v>4</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="28" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="15">
+      <c r="B11" s="14">
         <v>5</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="15" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="42" t="s">
         <v>241</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="34"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="43"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="19">
+      <c r="B14" s="18">
         <v>1</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="16" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="12">
+      <c r="B15" s="11">
         <v>2</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="16" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="12">
+      <c r="B16" s="11">
         <v>3</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="16" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="15">
+      <c r="B17" s="14">
         <v>4</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="17" t="s">
         <v>250</v>
       </c>
     </row>
@@ -4994,177 +5004,177 @@
   <sheetData>
     <row r="1" spans="2:5" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="44" t="s">
         <v>252</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="41" t="s">
+      <c r="C2" s="45"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="50" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="38"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="42"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="2:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>259</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="42" t="s">
         <v>253</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="43"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="19">
+      <c r="B8" s="18">
         <v>1</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="12">
+      <c r="B9" s="11">
         <v>2</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="17" t="s">
+      <c r="D9" s="11"/>
+      <c r="E9" s="16" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <v>3</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="17" t="s">
+      <c r="D10" s="11"/>
+      <c r="E10" s="16" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="12">
+      <c r="B11" s="11">
         <v>4</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="17" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="16" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="15">
+      <c r="B12" s="14">
         <v>5</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="18" t="s">
+      <c r="D12" s="14"/>
+      <c r="E12" s="17" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="42" t="s">
         <v>254</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="34"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="43"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="19">
+      <c r="B15" s="18">
         <v>1</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="16" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="12">
+      <c r="B16" s="11">
         <v>2</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="16" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="12">
+      <c r="B17" s="11">
         <v>3</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="16" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="15">
+      <c r="B18" s="14">
         <v>4</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="17" t="s">
         <v>269</v>
       </c>
     </row>
@@ -5199,124 +5209,124 @@
   <sheetData>
     <row r="1" spans="2:5" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="44" t="s">
         <v>271</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="41" t="s">
+      <c r="C2" s="45"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="50" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="38"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="42"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="2:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>259</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="42" t="s">
         <v>280</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="43"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="19">
+      <c r="B8" s="18">
         <v>1</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="12">
+      <c r="B9" s="11">
         <v>2</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="25" t="s">
+      <c r="D9" s="11"/>
+      <c r="E9" s="24" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <v>3</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="17" t="s">
+      <c r="D10" s="11"/>
+      <c r="E10" s="16" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="12">
+      <c r="B11" s="11">
         <v>4</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="17" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="16" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="26">
+      <c r="B12" s="25">
         <v>5</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="26" t="s">
         <v>226</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="28" t="s">
+      <c r="D12" s="25"/>
+      <c r="E12" s="27" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="15">
+      <c r="B13" s="14">
         <v>5</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="17" t="s">
         <v>277</v>
       </c>
     </row>
@@ -5338,10 +5348,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="B3:I15"/>
+  <dimension ref="B3:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5355,15 +5365,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="39" t="s">
         <v>285</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="39" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="39" t="s">
         <v>284</v>
       </c>
       <c r="C4" t="s">
@@ -5372,13 +5382,13 @@
       <c r="D4" t="s">
         <v>141</v>
       </c>
-      <c r="G4" s="52" t="s">
+      <c r="G4" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="H4" s="52" t="s">
+      <c r="H4" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="I4" s="52" t="s">
+      <c r="I4" s="40" t="s">
         <v>141</v>
       </c>
     </row>
@@ -5386,10 +5396,10 @@
       <c r="B5" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C5" s="51">
+      <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="51">
+      <c r="D5">
         <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -5408,10 +5418,10 @@
       <c r="B6" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C6" s="51">
+      <c r="C6">
         <v>6</v>
       </c>
-      <c r="D6" s="51">
+      <c r="D6">
         <v>2</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -5430,10 +5440,10 @@
       <c r="B7" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C7" s="51">
+      <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="51">
+      <c r="D7">
         <v>2</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -5452,8 +5462,7 @@
       <c r="B8" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51">
+      <c r="D8">
         <v>2</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -5472,10 +5481,10 @@
       <c r="B9" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C9" s="51">
+      <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" s="51">
+      <c r="D9">
         <v>6</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -5494,10 +5503,10 @@
       <c r="B10" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C10" s="51">
+      <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" s="51">
+      <c r="D10">
         <v>4</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -5516,10 +5525,10 @@
       <c r="B11" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C11" s="51">
+      <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11" s="51">
+      <c r="D11">
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -5538,10 +5547,9 @@
       <c r="B12" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C12" s="51">
+      <c r="C12">
         <v>3</v>
       </c>
-      <c r="D12" s="51"/>
       <c r="G12" s="2" t="s">
         <v>158</v>
       </c>
@@ -5558,10 +5566,10 @@
       <c r="B13" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C13" s="51">
+      <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" s="51">
+      <c r="D13">
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -5580,10 +5588,10 @@
       <c r="B14" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="51">
+      <c r="C14">
         <v>3</v>
       </c>
-      <c r="D14" s="51">
+      <c r="D14">
         <v>2</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -5602,10 +5610,10 @@
       <c r="B15" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C15" s="51">
+      <c r="C15">
         <v>4</v>
       </c>
-      <c r="D15" s="51">
+      <c r="D15">
         <v>3</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -5618,6 +5626,11 @@
       <c r="I15" s="2">
         <f>COUNTIFS(SPORTSMEN!$K$2:$K$51,ANALYSIS!$G15,SPORTSMEN!$I$2:$I$51,ANALYSIS!I$4)</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>424</v>
       </c>
     </row>
   </sheetData>
@@ -5632,7 +5645,7 @@
   </sheetPr>
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
@@ -5651,7 +5664,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="39" t="s">
         <v>237</v>
       </c>
       <c r="B1" t="s">
@@ -5659,33 +5672,33 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="39" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="39" t="s">
         <v>220</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="39" t="s">
         <v>227</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="H3" s="50" t="s">
+      <c r="H3" s="39" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="53">
+      <c r="A4" s="41">
         <v>1</v>
       </c>
       <c r="B4" t="s">
@@ -5711,7 +5724,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="53">
+      <c r="A5" s="41">
         <v>2</v>
       </c>
       <c r="B5" t="s">
@@ -5737,7 +5750,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="53">
+      <c r="A6" s="41">
         <v>3</v>
       </c>
       <c r="B6" t="s">
@@ -5763,7 +5776,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="53">
+      <c r="A7" s="41">
         <v>4</v>
       </c>
       <c r="B7" t="s">
@@ -5789,7 +5802,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="53">
+      <c r="A8" s="41">
         <v>5</v>
       </c>
       <c r="B8" t="s">
@@ -5815,7 +5828,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="53">
+      <c r="A9" s="41">
         <v>6</v>
       </c>
       <c r="B9" t="s">
@@ -5841,7 +5854,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="53">
+      <c r="A10" s="41">
         <v>7</v>
       </c>
       <c r="B10" t="s">
@@ -5867,7 +5880,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="53">
+      <c r="A11" s="41">
         <v>8</v>
       </c>
       <c r="B11" t="s">
@@ -5893,7 +5906,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="53">
+      <c r="A12" s="41">
         <v>9</v>
       </c>
       <c r="B12" t="s">
@@ -5919,7 +5932,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="53">
+      <c r="A13" s="41">
         <v>10</v>
       </c>
       <c r="B13" t="s">
@@ -5945,7 +5958,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="53">
+      <c r="A14" s="41">
         <v>11</v>
       </c>
       <c r="B14" t="s">
@@ -5971,7 +5984,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="53">
+      <c r="A15" s="41">
         <v>12</v>
       </c>
       <c r="B15" t="s">
@@ -5997,7 +6010,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="53">
+      <c r="A16" s="41">
         <v>13</v>
       </c>
       <c r="B16" t="s">
@@ -6023,7 +6036,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="53">
+      <c r="A17" s="41">
         <v>14</v>
       </c>
       <c r="B17" t="s">
@@ -6049,7 +6062,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="53">
+      <c r="A18" s="41">
         <v>15</v>
       </c>
       <c r="B18" t="s">
@@ -6075,7 +6088,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="53">
+      <c r="A19" s="41">
         <v>16</v>
       </c>
       <c r="B19" t="s">
@@ -6101,7 +6114,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="53">
+      <c r="A20" s="41">
         <v>17</v>
       </c>
       <c r="B20" t="s">
@@ -6127,7 +6140,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="53">
+      <c r="A21" s="41">
         <v>18</v>
       </c>
       <c r="B21" t="s">
@@ -6153,7 +6166,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="53">
+      <c r="A22" s="41">
         <v>19</v>
       </c>
       <c r="B22" t="s">
@@ -6179,7 +6192,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="53">
+      <c r="A23" s="41">
         <v>20</v>
       </c>
       <c r="B23" t="s">
@@ -6205,7 +6218,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="53">
+      <c r="A24" s="41">
         <v>21</v>
       </c>
       <c r="B24" t="s">
@@ -6231,7 +6244,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="53">
+      <c r="A25" s="41">
         <v>22</v>
       </c>
       <c r="B25" t="s">
@@ -6257,7 +6270,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="53">
+      <c r="A26" s="41">
         <v>23</v>
       </c>
       <c r="B26" t="s">
@@ -6283,7 +6296,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="53">
+      <c r="A27" s="41">
         <v>24</v>
       </c>
       <c r="B27" t="s">
@@ -6309,7 +6322,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="53">
+      <c r="A28" s="41">
         <v>25</v>
       </c>
       <c r="B28" t="s">
@@ -6335,7 +6348,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="53">
+      <c r="A29" s="41">
         <v>26</v>
       </c>
       <c r="B29" t="s">
@@ -6361,7 +6374,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="53">
+      <c r="A30" s="41">
         <v>27</v>
       </c>
       <c r="B30" t="s">
@@ -6387,7 +6400,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="53">
+      <c r="A31" s="41">
         <v>28</v>
       </c>
       <c r="B31" t="s">
@@ -6413,7 +6426,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="53">
+      <c r="A32" s="41">
         <v>29</v>
       </c>
       <c r="B32" t="s">
@@ -6439,7 +6452,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="53">
+      <c r="A33" s="41">
         <v>30</v>
       </c>
       <c r="B33" t="s">
@@ -6465,7 +6478,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="53">
+      <c r="A34" s="41">
         <v>31</v>
       </c>
       <c r="B34" t="s">
@@ -6491,7 +6504,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="53">
+      <c r="A35" s="41">
         <v>32</v>
       </c>
       <c r="B35" t="s">
@@ -6517,7 +6530,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="53">
+      <c r="A36" s="41">
         <v>33</v>
       </c>
       <c r="B36" t="s">
@@ -6543,7 +6556,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="53">
+      <c r="A37" s="41">
         <v>34</v>
       </c>
       <c r="B37" t="s">
@@ -6569,7 +6582,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="53">
+      <c r="A38" s="41">
         <v>35</v>
       </c>
       <c r="B38" t="s">
@@ -6595,7 +6608,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="53">
+      <c r="A39" s="41">
         <v>36</v>
       </c>
       <c r="B39" t="s">
@@ -6621,7 +6634,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="53">
+      <c r="A40" s="41">
         <v>37</v>
       </c>
       <c r="B40" t="s">
@@ -6647,7 +6660,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="53">
+      <c r="A41" s="41">
         <v>38</v>
       </c>
       <c r="B41" t="s">
@@ -6673,7 +6686,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="53">
+      <c r="A42" s="41">
         <v>39</v>
       </c>
       <c r="B42" t="s">
@@ -6699,7 +6712,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="53">
+      <c r="A43" s="41">
         <v>40</v>
       </c>
       <c r="B43" t="s">
@@ -6725,7 +6738,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="53">
+      <c r="A44" s="41">
         <v>41</v>
       </c>
       <c r="B44" t="s">
@@ -6751,7 +6764,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="53">
+      <c r="A45" s="41">
         <v>42</v>
       </c>
       <c r="B45" t="s">
@@ -6777,7 +6790,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="53">
+      <c r="A46" s="41">
         <v>43</v>
       </c>
       <c r="B46" t="s">
@@ -6803,7 +6816,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="53">
+      <c r="A47" s="41">
         <v>44</v>
       </c>
       <c r="B47" t="s">
@@ -6829,7 +6842,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="53">
+      <c r="A48" s="41">
         <v>45</v>
       </c>
       <c r="B48" t="s">
@@ -6855,7 +6868,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="53">
+      <c r="A49" s="41">
         <v>46</v>
       </c>
       <c r="B49" t="s">
@@ -6881,7 +6894,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="53">
+      <c r="A50" s="41">
         <v>47</v>
       </c>
       <c r="B50" t="s">
@@ -6907,7 +6920,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="53">
+      <c r="A51" s="41">
         <v>48</v>
       </c>
       <c r="B51" t="s">
@@ -6933,7 +6946,7 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="53">
+      <c r="A52" s="41">
         <v>49</v>
       </c>
       <c r="B52" t="s">
@@ -6959,7 +6972,7 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="53">
+      <c r="A53" s="41">
         <v>50</v>
       </c>
       <c r="B53" t="s">
@@ -7011,7 +7024,7 @@
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" style="24" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="23" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" customWidth="1"/>
     <col min="9" max="9" width="9.140625" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -7030,7 +7043,7 @@
       <c r="A1" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>220</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -7045,7 +7058,7 @@
       <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="33" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="5" t="s">
@@ -7066,7 +7079,7 @@
       <c r="M1" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>245</v>
       </c>
       <c r="O1" s="5" t="s">
@@ -7086,7 +7099,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="43">
+      <c r="A2" s="32">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="str">
@@ -7103,7 +7116,7 @@
       <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="45">
+      <c r="G2" s="34">
         <v>35699</v>
       </c>
       <c r="H2" s="3" t="s">
@@ -7127,7 +7140,7 @@
         <f>LOWER(CONCATENATE(F2,".",D2,"@",IF(L2="English",".org",".com")))</f>
         <v>abbott.annie@.org</v>
       </c>
-      <c r="N2" s="48">
+      <c r="N2" s="37">
         <v>94</v>
       </c>
       <c r="O2" s="3" t="s">
@@ -7143,12 +7156,12 @@
       <c r="R2" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="S2" s="49">
+      <c r="S2" s="38">
         <v>80727</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="43">
+      <c r="A3" s="32">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="str">
@@ -7165,7 +7178,7 @@
       <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="45">
+      <c r="G3" s="34">
         <v>33641</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -7189,7 +7202,7 @@
         <f t="shared" ref="M3:M51" si="1">LOWER(CONCATENATE(F3,".",D3,"@",IF(L3="English",".org",".com")))</f>
         <v>liesuchke.aurelie@.org</v>
       </c>
-      <c r="N3" s="48">
+      <c r="N3" s="37">
         <v>84.2</v>
       </c>
       <c r="O3" s="2" t="s">
@@ -7205,12 +7218,12 @@
       <c r="R3" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="S3" s="49">
+      <c r="S3" s="38">
         <v>87471</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="43">
+      <c r="A4" s="32">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="str">
@@ -7229,7 +7242,7 @@
       <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="45">
+      <c r="G4" s="34">
         <v>25394</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -7253,7 +7266,7 @@
         <f t="shared" si="1"/>
         <v>filho.tomas@.com</v>
       </c>
-      <c r="N4" s="48">
+      <c r="N4" s="37">
         <v>52.9</v>
       </c>
       <c r="O4" s="2" t="s">
@@ -7269,12 +7282,12 @@
       <c r="R4" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="S4" s="49">
+      <c r="S4" s="38">
         <v>64724</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="43">
+      <c r="A5" s="32">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="str">
@@ -7291,7 +7304,7 @@
       <c r="F5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="45">
+      <c r="G5" s="34">
         <v>27532</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -7315,7 +7328,7 @@
         <f t="shared" si="1"/>
         <v>cruickshank.darby@.org</v>
       </c>
-      <c r="N5" s="48">
+      <c r="N5" s="37">
         <v>48.9</v>
       </c>
       <c r="O5" s="2" t="s">
@@ -7331,12 +7344,12 @@
       <c r="R5" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="S5" s="49">
+      <c r="S5" s="38">
         <v>110823</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="43">
+      <c r="A6" s="32">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="str">
@@ -7353,7 +7366,7 @@
       <c r="F6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="45">
+      <c r="G6" s="34">
         <v>25706</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -7377,7 +7390,7 @@
         <f t="shared" si="1"/>
         <v>borer.jaydon@.org</v>
       </c>
-      <c r="N6" s="48">
+      <c r="N6" s="37">
         <v>84.8</v>
       </c>
       <c r="O6" s="2" t="s">
@@ -7393,12 +7406,12 @@
       <c r="R6" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="S6" s="49">
+      <c r="S6" s="38">
         <v>56916</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="43">
+      <c r="A7" s="32">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="str">
@@ -7415,7 +7428,7 @@
       <c r="F7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="45">
+      <c r="G7" s="34">
         <v>33944</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -7439,7 +7452,7 @@
         <f t="shared" si="1"/>
         <v>lynch.moriah @.org</v>
       </c>
-      <c r="N7" s="48">
+      <c r="N7" s="37">
         <v>83.2</v>
       </c>
       <c r="O7" s="2" t="s">
@@ -7455,12 +7468,12 @@
       <c r="R7" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="S7" s="49">
+      <c r="S7" s="38">
         <v>51133</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="43">
+      <c r="A8" s="32">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="str">
@@ -7477,7 +7490,7 @@
       <c r="F8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="45">
+      <c r="G8" s="34">
         <v>36370</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -7501,7 +7514,7 @@
         <f t="shared" si="1"/>
         <v>eichmann.amiya@.org</v>
       </c>
-      <c r="N8" s="48">
+      <c r="N8" s="37">
         <v>61.1</v>
       </c>
       <c r="O8" s="2" t="s">
@@ -7517,12 +7530,12 @@
       <c r="R8" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="S8" s="49">
+      <c r="S8" s="38">
         <v>65465</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="43">
+      <c r="A9" s="32">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="str">
@@ -7539,7 +7552,7 @@
       <c r="F9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="45">
+      <c r="G9" s="34">
         <v>23141</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -7563,7 +7576,7 @@
         <f t="shared" si="1"/>
         <v>rau.pierce@.org</v>
       </c>
-      <c r="N9" s="48">
+      <c r="N9" s="37">
         <v>105.7</v>
       </c>
       <c r="O9" s="2" t="s">
@@ -7579,12 +7592,12 @@
       <c r="R9" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="S9" s="49">
+      <c r="S9" s="38">
         <v>109885</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="43">
+      <c r="A10" s="32">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="str">
@@ -7601,7 +7614,7 @@
       <c r="F10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="45">
+      <c r="G10" s="34">
         <v>25965</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -7625,7 +7638,7 @@
         <f t="shared" si="1"/>
         <v>stevens.amelia@.org</v>
       </c>
-      <c r="N10" s="48">
+      <c r="N10" s="37">
         <v>65.3</v>
       </c>
       <c r="O10" s="2" t="s">
@@ -7641,12 +7654,12 @@
       <c r="R10" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="S10" s="49">
+      <c r="S10" s="38">
         <v>60061</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="43">
+      <c r="A11" s="32">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="str">
@@ -7663,7 +7676,7 @@
       <c r="F11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="45">
+      <c r="G11" s="34">
         <v>23732</v>
       </c>
       <c r="H11" s="2" t="s">
@@ -7687,7 +7700,7 @@
         <f t="shared" si="1"/>
         <v>simpson.toby@.org</v>
       </c>
-      <c r="N11" s="48">
+      <c r="N11" s="37">
         <v>62.9</v>
       </c>
       <c r="O11" s="2" t="s">
@@ -7703,12 +7716,12 @@
       <c r="R11" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="S11" s="49">
+      <c r="S11" s="38">
         <v>32758</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="43">
+      <c r="A12" s="32">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="str">
@@ -7725,7 +7738,7 @@
       <c r="F12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="45">
+      <c r="G12" s="34">
         <v>31733</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -7749,7 +7762,7 @@
         <f t="shared" si="1"/>
         <v>murphy.ethan@.org</v>
       </c>
-      <c r="N12" s="48">
+      <c r="N12" s="37">
         <v>104.3</v>
       </c>
       <c r="O12" s="2" t="s">
@@ -7765,12 +7778,12 @@
       <c r="R12" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="S12" s="49">
+      <c r="S12" s="38">
         <v>99613</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="43">
+      <c r="A13" s="32">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="str">
@@ -7787,7 +7800,7 @@
       <c r="F13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="45">
+      <c r="G13" s="34">
         <v>28412</v>
       </c>
       <c r="H13" s="2" t="s">
@@ -7811,7 +7824,7 @@
         <f t="shared" si="1"/>
         <v>wood.ashley@.org</v>
       </c>
-      <c r="N13" s="48">
+      <c r="N13" s="37">
         <v>100.7</v>
       </c>
       <c r="O13" s="2" t="s">
@@ -7827,12 +7840,12 @@
       <c r="R13" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="S13" s="49">
+      <c r="S13" s="38">
         <v>56595</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="43">
+      <c r="A14" s="32">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="str">
@@ -7849,7 +7862,7 @@
       <c r="F14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="45">
+      <c r="G14" s="34">
         <v>28168</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -7873,7 +7886,7 @@
         <f t="shared" si="1"/>
         <v>scott.megan@.org</v>
       </c>
-      <c r="N14" s="48">
+      <c r="N14" s="37">
         <v>70.900000000000006</v>
       </c>
       <c r="O14" s="2" t="s">
@@ -7889,12 +7902,12 @@
       <c r="R14" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="S14" s="49">
+      <c r="S14" s="38">
         <v>117408</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="43">
+      <c r="A15" s="32">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="str">
@@ -7911,7 +7924,7 @@
       <c r="F15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="45">
+      <c r="G15" s="34">
         <v>21788</v>
       </c>
       <c r="H15" s="2" t="s">
@@ -7935,7 +7948,7 @@
         <f t="shared" si="1"/>
         <v>weinhae.helmut@.com</v>
       </c>
-      <c r="N15" s="48">
+      <c r="N15" s="37">
         <v>68.3</v>
       </c>
       <c r="O15" s="2" t="s">
@@ -7951,12 +7964,12 @@
       <c r="R15" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="S15" s="49">
+      <c r="S15" s="38">
         <v>64862</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="43">
+      <c r="A16" s="32">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="str">
@@ -7973,7 +7986,7 @@
       <c r="F16" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="G16" s="45">
+      <c r="G16" s="34">
         <v>23804</v>
       </c>
       <c r="H16" s="2" t="s">
@@ -7997,7 +8010,7 @@
         <f t="shared" si="1"/>
         <v>`.milena@.com</v>
       </c>
-      <c r="N16" s="48">
+      <c r="N16" s="37">
         <v>105.3</v>
       </c>
       <c r="O16" s="2" t="s">
@@ -8013,12 +8026,12 @@
       <c r="R16" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="S16" s="49">
+      <c r="S16" s="38">
         <v>10241</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="43">
+      <c r="A17" s="32">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="str">
@@ -8035,7 +8048,7 @@
       <c r="F17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="45">
+      <c r="G17" s="34">
         <v>25405</v>
       </c>
       <c r="H17" s="2" t="s">
@@ -8059,7 +8072,7 @@
         <f t="shared" si="1"/>
         <v>birnbaum.lothar@.com</v>
       </c>
-      <c r="N17" s="48">
+      <c r="N17" s="37">
         <v>48.6</v>
       </c>
       <c r="O17" s="2" t="s">
@@ -8075,12 +8088,12 @@
       <c r="R17" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="S17" s="49">
+      <c r="S17" s="38">
         <v>88762</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="43">
+      <c r="A18" s="32">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="str">
@@ -8097,7 +8110,7 @@
       <c r="F18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G18" s="45">
+      <c r="G18" s="34">
         <v>26582</v>
       </c>
       <c r="H18" s="2" t="s">
@@ -8121,7 +8134,7 @@
         <f t="shared" si="1"/>
         <v>stolze.pietro@.com</v>
       </c>
-      <c r="N18" s="48">
+      <c r="N18" s="37">
         <v>105.9</v>
       </c>
       <c r="O18" s="2" t="s">
@@ -8137,12 +8150,12 @@
       <c r="R18" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="S18" s="49">
+      <c r="S18" s="38">
         <v>80757</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="43">
+      <c r="A19" s="32">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="str">
@@ -8159,7 +8172,7 @@
       <c r="F19" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G19" s="47">
+      <c r="G19" s="36">
         <v>21793</v>
       </c>
       <c r="H19" s="2" t="s">
@@ -8183,7 +8196,7 @@
         <f t="shared" si="1"/>
         <v>tlustek.richard @.com</v>
       </c>
-      <c r="N19" s="48">
+      <c r="N19" s="37">
         <v>71.099999999999994</v>
       </c>
       <c r="O19" s="2" t="s">
@@ -8199,12 +8212,12 @@
       <c r="R19" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="S19" s="49">
+      <c r="S19" s="38">
         <v>88794</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="43">
+      <c r="A20" s="32">
         <v>19</v>
       </c>
       <c r="B20" s="3" t="str">
@@ -8221,7 +8234,7 @@
       <c r="F20" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G20" s="47">
+      <c r="G20" s="36">
         <v>28262</v>
       </c>
       <c r="H20" s="2" t="s">
@@ -8245,7 +8258,7 @@
         <f t="shared" si="1"/>
         <v>raynor.earnestine@.org</v>
       </c>
-      <c r="N20" s="48">
+      <c r="N20" s="37">
         <v>70.3</v>
       </c>
       <c r="O20" s="2" t="s">
@@ -8261,12 +8274,12 @@
       <c r="R20" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="S20" s="49">
+      <c r="S20" s="38">
         <v>63526</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="43">
+      <c r="A21" s="32">
         <v>20</v>
       </c>
       <c r="B21" s="3" t="str">
@@ -8283,7 +8296,7 @@
       <c r="F21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G21" s="47">
+      <c r="G21" s="36">
         <v>27767</v>
       </c>
       <c r="H21" s="2" t="s">
@@ -8307,7 +8320,7 @@
         <f t="shared" si="1"/>
         <v>gaylord.jason@.org</v>
       </c>
-      <c r="N21" s="48">
+      <c r="N21" s="37">
         <v>54.7</v>
       </c>
       <c r="O21" s="2" t="s">
@@ -8323,12 +8336,12 @@
       <c r="R21" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="S21" s="49">
+      <c r="S21" s="38">
         <v>46352</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="43">
+      <c r="A22" s="32">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="str">
@@ -8345,7 +8358,7 @@
       <c r="F22" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G22" s="47">
+      <c r="G22" s="36">
         <v>35268</v>
       </c>
       <c r="H22" s="2" t="s">
@@ -8369,7 +8382,7 @@
         <f t="shared" si="1"/>
         <v>sauer.kendrick@.org</v>
       </c>
-      <c r="N22" s="48">
+      <c r="N22" s="37">
         <v>100.9</v>
       </c>
       <c r="O22" s="2" t="s">
@@ -8385,12 +8398,12 @@
       <c r="R22" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="S22" s="49">
+      <c r="S22" s="38">
         <v>106808</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="43">
+      <c r="A23" s="32">
         <v>22</v>
       </c>
       <c r="B23" s="3" t="str">
@@ -8407,7 +8420,7 @@
       <c r="F23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G23" s="47">
+      <c r="G23" s="36">
         <v>23483</v>
       </c>
       <c r="H23" s="2" t="s">
@@ -8431,7 +8444,7 @@
         <f t="shared" si="1"/>
         <v>olson.annabell@.org</v>
       </c>
-      <c r="N23" s="48">
+      <c r="N23" s="37">
         <v>84.3</v>
       </c>
       <c r="O23" s="2" t="s">
@@ -8447,12 +8460,12 @@
       <c r="R23" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="S23" s="49">
+      <c r="S23" s="38">
         <v>96468</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="43">
+      <c r="A24" s="32">
         <v>23</v>
       </c>
       <c r="B24" s="3" t="str">
@@ -8469,7 +8482,7 @@
       <c r="F24" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="G24" s="47">
+      <c r="G24" s="36">
         <v>20437</v>
       </c>
       <c r="H24" s="2" t="s">
@@ -8493,7 +8506,7 @@
         <f t="shared" si="1"/>
         <v>upton.jena@.org</v>
       </c>
-      <c r="N24" s="48">
+      <c r="N24" s="37">
         <v>66.8</v>
       </c>
       <c r="O24" s="2" t="s">
@@ -8509,12 +8522,12 @@
       <c r="R24" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S24" s="49">
+      <c r="S24" s="38">
         <v>16526</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="43">
+      <c r="A25" s="32">
         <v>24</v>
       </c>
       <c r="B25" s="3" t="str">
@@ -8531,7 +8544,7 @@
       <c r="F25" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G25" s="47">
+      <c r="G25" s="36">
         <v>36400</v>
       </c>
       <c r="H25" s="2" t="s">
@@ -8555,7 +8568,7 @@
         <f t="shared" si="1"/>
         <v>bins.shanny@.org</v>
       </c>
-      <c r="N25" s="48">
+      <c r="N25" s="37">
         <v>59.4</v>
       </c>
       <c r="O25" s="2" t="s">
@@ -8571,12 +8584,12 @@
       <c r="R25" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="S25" s="49">
+      <c r="S25" s="38">
         <v>21891</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="43">
+      <c r="A26" s="32">
         <v>25</v>
       </c>
       <c r="B26" s="3" t="str">
@@ -8593,7 +8606,7 @@
       <c r="F26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G26" s="47">
+      <c r="G26" s="36">
         <v>24309</v>
       </c>
       <c r="H26" s="2" t="s">
@@ -8617,7 +8630,7 @@
         <f t="shared" si="1"/>
         <v>abshire.tia@.org</v>
       </c>
-      <c r="N26" s="48">
+      <c r="N26" s="37">
         <v>77.8</v>
       </c>
       <c r="O26" s="2" t="s">
@@ -8633,12 +8646,12 @@
       <c r="R26" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="S26" s="49">
+      <c r="S26" s="38">
         <v>62037</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="43">
+      <c r="A27" s="32">
         <v>26</v>
       </c>
       <c r="B27" s="3" t="str">
@@ -8655,7 +8668,7 @@
       <c r="F27" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G27" s="47">
+      <c r="G27" s="36">
         <v>28570</v>
       </c>
       <c r="H27" s="2" t="s">
@@ -8679,7 +8692,7 @@
         <f t="shared" si="1"/>
         <v>runolfsdottir.isabel@.org</v>
       </c>
-      <c r="N27" s="48">
+      <c r="N27" s="37">
         <v>85.9</v>
       </c>
       <c r="O27" s="2" t="s">
@@ -8695,12 +8708,12 @@
       <c r="R27" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="S27" s="49">
+      <c r="S27" s="38">
         <v>89737</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="43">
+      <c r="A28" s="32">
         <v>27</v>
       </c>
       <c r="B28" s="3" t="str">
@@ -8717,7 +8730,7 @@
       <c r="F28" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G28" s="47">
+      <c r="G28" s="36">
         <v>25767</v>
       </c>
       <c r="H28" s="2" t="s">
@@ -8741,7 +8754,7 @@
         <f t="shared" si="1"/>
         <v>wesack.barney@.com</v>
       </c>
-      <c r="N28" s="48">
+      <c r="N28" s="37">
         <v>93.4</v>
       </c>
       <c r="O28" s="2" t="s">
@@ -8757,12 +8770,12 @@
       <c r="R28" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="S28" s="49">
+      <c r="S28" s="38">
         <v>41039</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="43">
+      <c r="A29" s="32">
         <v>28</v>
       </c>
       <c r="B29" s="3" t="str">
@@ -8779,7 +8792,7 @@
       <c r="F29" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G29" s="47">
+      <c r="G29" s="36">
         <v>30020</v>
       </c>
       <c r="H29" s="2" t="s">
@@ -8803,7 +8816,7 @@
         <f t="shared" si="1"/>
         <v>kade.baruch@.com</v>
       </c>
-      <c r="N29" s="48">
+      <c r="N29" s="37">
         <v>95.5</v>
       </c>
       <c r="O29" s="2" t="s">
@@ -8819,12 +8832,12 @@
       <c r="R29" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="S29" s="49">
+      <c r="S29" s="38">
         <v>28458</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="43">
+      <c r="A30" s="32">
         <v>29</v>
       </c>
       <c r="B30" s="3" t="str">
@@ -8841,7 +8854,7 @@
       <c r="F30" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G30" s="47">
+      <c r="G30" s="36">
         <v>34361</v>
       </c>
       <c r="H30" s="2" t="s">
@@ -8865,7 +8878,7 @@
         <f t="shared" si="1"/>
         <v>rosemann.liesbeth@.com</v>
       </c>
-      <c r="N30" s="48">
+      <c r="N30" s="37">
         <v>52.2</v>
       </c>
       <c r="O30" s="2" t="s">
@@ -8881,12 +8894,12 @@
       <c r="R30" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="S30" s="49">
+      <c r="S30" s="38">
         <v>55007</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="43">
+      <c r="A31" s="32">
         <v>30</v>
       </c>
       <c r="B31" s="3" t="str">
@@ -8903,7 +8916,7 @@
       <c r="F31" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G31" s="47">
+      <c r="G31" s="36">
         <v>29137</v>
       </c>
       <c r="H31" s="2" t="s">
@@ -8927,7 +8940,7 @@
         <f t="shared" si="1"/>
         <v>moreau.valentine@.com</v>
       </c>
-      <c r="N31" s="48">
+      <c r="N31" s="37">
         <v>74.599999999999994</v>
       </c>
       <c r="O31" s="2" t="s">
@@ -8943,12 +8956,12 @@
       <c r="R31" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="S31" s="49">
+      <c r="S31" s="38">
         <v>69041</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="43">
+      <c r="A32" s="32">
         <v>31</v>
       </c>
       <c r="B32" s="3" t="str">
@@ -8965,7 +8978,7 @@
       <c r="F32" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G32" s="46">
+      <c r="G32" s="35">
         <v>32867</v>
       </c>
       <c r="H32" s="2" t="s">
@@ -8989,7 +9002,7 @@
         <f t="shared" si="1"/>
         <v>durand.paulette@.com</v>
       </c>
-      <c r="N32" s="48">
+      <c r="N32" s="37">
         <v>81.7</v>
       </c>
       <c r="O32" s="2" t="s">
@@ -9005,12 +9018,12 @@
       <c r="R32" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="S32" s="49">
+      <c r="S32" s="38">
         <v>86262</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="43">
+      <c r="A33" s="32">
         <v>32</v>
       </c>
       <c r="B33" s="3" t="str">
@@ -9027,7 +9040,7 @@
       <c r="F33" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G33" s="46">
+      <c r="G33" s="35">
         <v>25925</v>
       </c>
       <c r="H33" s="2" t="s">
@@ -9051,7 +9064,7 @@
         <f t="shared" si="1"/>
         <v>chevalier.laure-alix@.com</v>
       </c>
-      <c r="N33" s="48">
+      <c r="N33" s="37">
         <v>78.099999999999994</v>
       </c>
       <c r="O33" s="2" t="s">
@@ -9067,12 +9080,12 @@
       <c r="R33" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S33" s="49">
+      <c r="S33" s="38">
         <v>19234</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="43">
+      <c r="A34" s="32">
         <v>33</v>
       </c>
       <c r="B34" s="3" t="str">
@@ -9089,7 +9102,7 @@
       <c r="F34" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G34" s="46">
+      <c r="G34" s="35">
         <v>29529</v>
       </c>
       <c r="H34" s="2" t="s">
@@ -9113,7 +9126,7 @@
         <f t="shared" si="1"/>
         <v>toussaint.claude@.com</v>
       </c>
-      <c r="N34" s="48">
+      <c r="N34" s="37">
         <v>57.1</v>
       </c>
       <c r="O34" s="2" t="s">
@@ -9129,12 +9142,12 @@
       <c r="R34" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="S34" s="49">
+      <c r="S34" s="38">
         <v>95123</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="43">
+      <c r="A35" s="32">
         <v>34</v>
       </c>
       <c r="B35" s="3" t="str">
@@ -9151,7 +9164,7 @@
       <c r="F35" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G35" s="46">
+      <c r="G35" s="35">
         <v>29875</v>
       </c>
       <c r="H35" s="2" t="s">
@@ -9175,7 +9188,7 @@
         <f t="shared" si="1"/>
         <v>lenoir.victor@.com</v>
       </c>
-      <c r="N35" s="48">
+      <c r="N35" s="37">
         <v>56</v>
       </c>
       <c r="O35" s="2" t="s">
@@ -9191,12 +9204,12 @@
       <c r="R35" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="S35" s="49">
+      <c r="S35" s="38">
         <v>62761</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="43">
+      <c r="A36" s="32">
         <v>35</v>
       </c>
       <c r="B36" s="3" t="str">
@@ -9213,7 +9226,7 @@
       <c r="F36" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G36" s="46">
+      <c r="G36" s="35">
         <v>20300</v>
       </c>
       <c r="H36" s="2" t="s">
@@ -9237,7 +9250,7 @@
         <f t="shared" si="1"/>
         <v>lenoir.arthur@.com</v>
       </c>
-      <c r="N36" s="48">
+      <c r="N36" s="37">
         <v>88.6</v>
       </c>
       <c r="O36" s="2" t="s">
@@ -9253,12 +9266,12 @@
       <c r="R36" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="S36" s="49">
+      <c r="S36" s="38">
         <v>108431</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="43">
+      <c r="A37" s="32">
         <v>36</v>
       </c>
       <c r="B37" s="3" t="str">
@@ -9275,7 +9288,7 @@
       <c r="F37" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G37" s="46">
+      <c r="G37" s="35">
         <v>27428</v>
       </c>
       <c r="H37" s="2" t="s">
@@ -9299,7 +9312,7 @@
         <f t="shared" si="1"/>
         <v>lebrun-brun.benjamin@.com</v>
       </c>
-      <c r="N37" s="48">
+      <c r="N37" s="37">
         <v>78.2</v>
       </c>
       <c r="O37" s="2" t="s">
@@ -9315,12 +9328,12 @@
       <c r="R37" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="S37" s="49">
+      <c r="S37" s="38">
         <v>66268</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38" s="43">
+      <c r="A38" s="32">
         <v>37</v>
       </c>
       <c r="B38" s="3" t="str">
@@ -9337,7 +9350,7 @@
       <c r="F38" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G38" s="46">
+      <c r="G38" s="35">
         <v>31585</v>
       </c>
       <c r="H38" s="2" t="s">
@@ -9361,7 +9374,7 @@
         <f t="shared" si="1"/>
         <v>maillard.antoine@.com</v>
       </c>
-      <c r="N38" s="48">
+      <c r="N38" s="37">
         <v>95.8</v>
       </c>
       <c r="O38" s="2" t="s">
@@ -9377,12 +9390,12 @@
       <c r="R38" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="S38" s="49">
+      <c r="S38" s="38">
         <v>33970</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="43">
+      <c r="A39" s="32">
         <v>38</v>
       </c>
       <c r="B39" s="3" t="str">
@@ -9399,7 +9412,7 @@
       <c r="F39" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G39" s="46">
+      <c r="G39" s="35">
         <v>30327</v>
       </c>
       <c r="H39" s="2" t="s">
@@ -9423,7 +9436,7 @@
         <f t="shared" si="1"/>
         <v>hoarau-guyon.bernard@.com</v>
       </c>
-      <c r="N39" s="48">
+      <c r="N39" s="37">
         <v>59.7</v>
       </c>
       <c r="O39" s="2" t="s">
@@ -9439,12 +9452,12 @@
       <c r="R39" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="S39" s="49">
+      <c r="S39" s="38">
         <v>71352</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="43">
+      <c r="A40" s="32">
         <v>39</v>
       </c>
       <c r="B40" s="3" t="str">
@@ -9463,7 +9476,7 @@
       <c r="F40" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G40" s="46">
+      <c r="G40" s="35">
         <v>31016</v>
       </c>
       <c r="H40" s="2" t="s">
@@ -9487,7 +9500,7 @@
         <f t="shared" si="1"/>
         <v>tercero.hidalgo@.com</v>
       </c>
-      <c r="N40" s="48">
+      <c r="N40" s="37">
         <v>77.7</v>
       </c>
       <c r="O40" s="2" t="s">
@@ -9503,12 +9516,12 @@
       <c r="R40" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="S40" s="49">
+      <c r="S40" s="38">
         <v>116376</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A41" s="43">
+      <c r="A41" s="32">
         <v>40</v>
       </c>
       <c r="B41" s="3" t="str">
@@ -9525,7 +9538,7 @@
       <c r="F41" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G41" s="46">
+      <c r="G41" s="35">
         <v>32314</v>
       </c>
       <c r="H41" s="2" t="s">
@@ -9549,7 +9562,7 @@
         <f t="shared" si="1"/>
         <v>polanco.hadalgo@.com</v>
       </c>
-      <c r="N41" s="48">
+      <c r="N41" s="37">
         <v>98</v>
       </c>
       <c r="O41" s="2" t="s">
@@ -9565,12 +9578,12 @@
       <c r="R41" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S41" s="49">
+      <c r="S41" s="38">
         <v>114144</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" s="43">
+      <c r="A42" s="32">
         <v>41</v>
       </c>
       <c r="B42" s="3" t="str">
@@ -9587,7 +9600,7 @@
       <c r="F42" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G42" s="46">
+      <c r="G42" s="35">
         <v>27076</v>
       </c>
       <c r="H42" s="2" t="s">
@@ -9611,7 +9624,7 @@
         <f t="shared" si="1"/>
         <v>oliviera.laura@.com</v>
       </c>
-      <c r="N42" s="48">
+      <c r="N42" s="37">
         <v>51.9</v>
       </c>
       <c r="O42" s="2" t="s">
@@ -9627,12 +9640,12 @@
       <c r="R42" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="S42" s="49">
+      <c r="S42" s="38">
         <v>79872</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A43" s="43">
+      <c r="A43" s="32">
         <v>42</v>
       </c>
       <c r="B43" s="3" t="str">
@@ -9649,7 +9662,7 @@
       <c r="F43" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G43" s="46">
+      <c r="G43" s="35">
         <v>32941</v>
       </c>
       <c r="H43" s="2" t="s">
@@ -9673,7 +9686,7 @@
         <f t="shared" si="1"/>
         <v>garza.ainhoa@.com</v>
       </c>
-      <c r="N43" s="48">
+      <c r="N43" s="37">
         <v>55.6</v>
       </c>
       <c r="O43" s="2" t="s">
@@ -9689,12 +9702,12 @@
       <c r="R43" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="S43" s="49">
+      <c r="S43" s="38">
         <v>101969</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A44" s="43">
+      <c r="A44" s="32">
         <v>43</v>
       </c>
       <c r="B44" s="3" t="str">
@@ -9711,7 +9724,7 @@
       <c r="F44" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="G44" s="46">
+      <c r="G44" s="35">
         <v>21927</v>
       </c>
       <c r="H44" s="2" t="s">
@@ -9735,7 +9748,7 @@
         <f t="shared" si="1"/>
         <v>banda.isabel@.com</v>
       </c>
-      <c r="N44" s="48">
+      <c r="N44" s="37">
         <v>102.3</v>
       </c>
       <c r="O44" s="2" t="s">
@@ -9751,12 +9764,12 @@
       <c r="R44" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="S44" s="49">
+      <c r="S44" s="38">
         <v>50659</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A45" s="43">
+      <c r="A45" s="32">
         <v>44</v>
       </c>
       <c r="B45" s="3" t="str">
@@ -9773,7 +9786,7 @@
       <c r="F45" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="G45" s="46">
+      <c r="G45" s="35">
         <v>23952</v>
       </c>
       <c r="H45" s="2" t="s">
@@ -9797,7 +9810,7 @@
         <f t="shared" si="1"/>
         <v>mateos.carolota@.com</v>
       </c>
-      <c r="N45" s="48">
+      <c r="N45" s="37">
         <v>58.8</v>
       </c>
       <c r="O45" s="2" t="s">
@@ -9813,12 +9826,12 @@
       <c r="R45" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="S45" s="49">
+      <c r="S45" s="38">
         <v>58215</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A46" s="43">
+      <c r="A46" s="32">
         <v>45</v>
       </c>
       <c r="B46" s="3" t="str">
@@ -9835,7 +9848,7 @@
       <c r="F46" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="G46" s="46">
+      <c r="G46" s="35">
         <v>22044</v>
       </c>
       <c r="H46" s="2" t="s">
@@ -9859,7 +9872,7 @@
         <f t="shared" si="1"/>
         <v>prins.elize@.com</v>
       </c>
-      <c r="N46" s="48">
+      <c r="N46" s="37">
         <v>63.8</v>
       </c>
       <c r="O46" s="2" t="s">
@@ -9875,12 +9888,12 @@
       <c r="R46" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="S46" s="49">
+      <c r="S46" s="38">
         <v>39935</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A47" s="43">
+      <c r="A47" s="32">
         <v>46</v>
       </c>
       <c r="B47" s="3" t="str">
@@ -9897,7 +9910,7 @@
       <c r="F47" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="G47" s="46">
+      <c r="G47" s="35">
         <v>26940</v>
       </c>
       <c r="H47" s="2" t="s">
@@ -9921,7 +9934,7 @@
         <f t="shared" si="1"/>
         <v>pham.ryan@.com</v>
       </c>
-      <c r="N47" s="48">
+      <c r="N47" s="37">
         <v>98.6</v>
       </c>
       <c r="O47" s="2" t="s">
@@ -9937,12 +9950,12 @@
       <c r="R47" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S47" s="49">
+      <c r="S47" s="38">
         <v>44865</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A48" s="43">
+      <c r="A48" s="32">
         <v>47</v>
       </c>
       <c r="B48" s="3" t="str">
@@ -9959,7 +9972,7 @@
       <c r="F48" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="G48" s="46">
+      <c r="G48" s="35">
         <v>24936</v>
       </c>
       <c r="H48" s="2" t="s">
@@ -9983,7 +9996,7 @@
         <f t="shared" si="1"/>
         <v>rotteveel.elise@.com</v>
       </c>
-      <c r="N48" s="48">
+      <c r="N48" s="37">
         <v>61.8</v>
       </c>
       <c r="O48" s="2" t="s">
@@ -9999,12 +10012,12 @@
       <c r="R48" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S48" s="49">
+      <c r="S48" s="38">
         <v>90478</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A49" s="43">
+      <c r="A49" s="32">
         <v>48</v>
       </c>
       <c r="B49" s="3" t="str">
@@ -10021,7 +10034,7 @@
       <c r="F49" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="G49" s="46">
+      <c r="G49" s="35">
         <v>35567</v>
       </c>
       <c r="H49" s="2" t="s">
@@ -10045,7 +10058,7 @@
         <f t="shared" si="1"/>
         <v>soderberg.mirjam@.com</v>
       </c>
-      <c r="N49" s="48">
+      <c r="N49" s="37">
         <v>50</v>
       </c>
       <c r="O49" s="2" t="s">
@@ -10061,12 +10074,12 @@
       <c r="R49" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="S49" s="49">
+      <c r="S49" s="38">
         <v>38965</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="43">
+      <c r="A50" s="32">
         <v>49</v>
       </c>
       <c r="B50" s="3" t="str">
@@ -10083,7 +10096,7 @@
       <c r="F50" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G50" s="46">
+      <c r="G50" s="35">
         <v>31832</v>
       </c>
       <c r="H50" s="2" t="s">
@@ -10107,7 +10120,7 @@
         <f t="shared" si="1"/>
         <v>palsson.berndt@.com</v>
       </c>
-      <c r="N50" s="48">
+      <c r="N50" s="37">
         <v>45.9</v>
       </c>
       <c r="O50" s="2" t="s">
@@ -10123,12 +10136,12 @@
       <c r="R50" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="S50" s="49">
+      <c r="S50" s="38">
         <v>35387</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A51" s="43">
+      <c r="A51" s="32">
         <v>50</v>
       </c>
       <c r="B51" s="3" t="str">
@@ -10147,7 +10160,7 @@
       <c r="F51" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G51" s="46">
+      <c r="G51" s="35">
         <v>34178</v>
       </c>
       <c r="H51" s="2" t="s">
@@ -10171,7 +10184,7 @@
         <f t="shared" si="1"/>
         <v>sobrinho.adriano@.com</v>
       </c>
-      <c r="N51" s="48">
+      <c r="N51" s="37">
         <v>92.5</v>
       </c>
       <c r="O51" s="2" t="s">
@@ -10187,7 +10200,7 @@
       <c r="R51" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="S51" s="49">
+      <c r="S51" s="38">
         <v>20532</v>
       </c>
     </row>
@@ -10225,266 +10238,266 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="30" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="31" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="31" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="31" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="31" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="31" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="31" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="31" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="31" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="31" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="31" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="31" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="31" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="31" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="31" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="31" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="31" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="31" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="31" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="31" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="31" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="31" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="31" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="31" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="31" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="31" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="31" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="B31" s="31" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="31" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="31" t="s">
         <v>205</v>
       </c>
     </row>
@@ -10513,7 +10526,7 @@
       <c r="A1" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>138</v>
       </c>
       <c r="C1" s="3" t="s">

</xml_diff>